<commit_message>
add GACS, 51.15.194.251, UAAV, HTW Chur, FORTH, Irstea (#65)
</commit_message>
<xml_diff>
--- a/django/bartocfast/fixtures/skosmosinstances.xlsx
+++ b/django/bartocfast/fixtures/skosmosinstances.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -89,16 +89,46 @@
     <t>timeout</t>
   </si>
   <si>
-    <t>server down 03.07.2019</t>
-  </si>
-  <si>
-    <t>too slow</t>
-  </si>
-  <si>
     <t>context</t>
   </si>
   <si>
     <t>wildcard</t>
+  </si>
+  <si>
+    <t>GACS</t>
+  </si>
+  <si>
+    <t>http://artemide.art.uniroma2.it/skosmos/</t>
+  </si>
+  <si>
+    <t>http://51.15.194.251/Skosmos/</t>
+  </si>
+  <si>
+    <t>https://voc.uni-ak.ac.at/skosmos</t>
+  </si>
+  <si>
+    <t>51.15.194.251</t>
+  </si>
+  <si>
+    <t>UAAV</t>
+  </si>
+  <si>
+    <t>http://skosmos.linkeddata.ch/</t>
+  </si>
+  <si>
+    <t>HTW Chur</t>
+  </si>
+  <si>
+    <t>https://isl.ics.forth.gr/apollonis-federated-thesaurus/</t>
+  </si>
+  <si>
+    <t>FORTH</t>
+  </si>
+  <si>
+    <t>https://vocabulaires.irstea.fr/skosmos/</t>
+  </si>
+  <si>
+    <t>Irstea</t>
   </si>
 </sst>
 </file>
@@ -426,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +471,7 @@
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,13 +479,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -483,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -497,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -511,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -519,13 +549,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -539,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -552,11 +582,8 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -570,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -583,8 +610,89 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>22</v>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dynamic JSON-LD output @API tab (#74)
* results replaces results_global

* api replaces data

* remove whitespaces from names

* dynamic JSON-LD output
</commit_message>
<xml_diff>
--- a/django/bartocfast/fixtures/skosmosinstances.xlsx
+++ b/django/bartocfast/fixtures/skosmosinstances.xlsx
@@ -110,9 +110,6 @@
     <t>http://skosmos.linkeddata.ch/</t>
   </si>
   <si>
-    <t>HTW Chur</t>
-  </si>
-  <si>
     <t>FORTH</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>http://thesaurus.web.ined.fr/navigateur</t>
+  </si>
+  <si>
+    <t>HTW-Chur</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -636,7 +636,7 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -675,10 +675,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -689,10 +689,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -703,10 +703,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Add Research Vocabularies Australia (#84)
* add models_ldapi

* Update __init__.py

* add ldapi_models

* add ldapiendpoints

* add populate_ldapiendpoints

* register Ldpai*

* fix typos

* add normalize_ldapi

* fix typo

* add LdapiEndpoint

* fix view logic

* add Helper methods

* update views.api

* fix choices

* houskeeping

* update html

* Update views.py

- context_value for graphene
- updated gather_requests and make_context to allow for RVA

* add slave context

* remove self check for disable

* add Helper.master/slave methods

* fix typos

* generalize functions

* Update add_resource.txt

* turn off debug

* update version

* add slave context

* add ScoLOMFR

* Update ldapiendpoints.xlsx
</commit_message>
<xml_diff>
--- a/django/bartocfast/fixtures/skosmosinstances.xlsx
+++ b/django/bartocfast/fixtures/skosmosinstances.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>http://skosmos.linkeddata.ch</t>
+  </si>
+  <si>
+    <t>ScoLOMFR</t>
+  </si>
+  <si>
+    <t>https://www.reseau-canope.fr/scolomfr/data</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,6 +721,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>